<commit_message>
ewakuacja ze starego laptopa
</commit_message>
<xml_diff>
--- a/Statystyki_2018/Template/oglr.xlsx
+++ b/Statystyki_2018/Template/oglr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\myProjects\prv\statystyki\Statystyki_2018\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E4CA76-C42A-4D89-B8A1-DADE61CFEEF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87CDC6C-F0DF-4E60-A93F-2DD9DE20B5A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-48" yWindow="-48" windowWidth="23136" windowHeight="12528" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-48" yWindow="-48" windowWidth="23136" windowHeight="12528" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="I" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">I!$A$1:$X$6</definedName>
   </definedNames>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -74,9 +74,6 @@
     <t>Pozostałość na koniec okresu kontrolnego</t>
   </si>
   <si>
-    <t>Wielkrotna</t>
-  </si>
-  <si>
     <t>Rozpraw</t>
   </si>
   <si>
@@ -156,13 +153,16 @@
   </si>
   <si>
     <t xml:space="preserve">Sprawozdanie z ruchu spraw </t>
+  </si>
+  <si>
+    <t>Wielokrotna</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -196,6 +196,12 @@
       <color rgb="FF000000"/>
       <name val="Czcionka tekstu podstawowego"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -217,7 +223,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -255,86 +261,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -345,62 +276,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -755,8 +666,8 @@
   </sheetPr>
   <dimension ref="B1:Z7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="Y3" sqref="Y3:Z6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -764,7 +675,7 @@
     <col min="1" max="1" width="1.59765625" customWidth="1"/>
     <col min="2" max="2" width="1.5" customWidth="1"/>
     <col min="3" max="3" width="31.8984375" customWidth="1"/>
-    <col min="4" max="4" width="20.09765625" customWidth="1"/>
+    <col min="4" max="4" width="36.296875" customWidth="1"/>
     <col min="5" max="24" width="5.5" customWidth="1"/>
     <col min="25" max="1015" width="8.5" customWidth="1"/>
   </cols>
@@ -773,7 +684,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="3"/>
@@ -790,7 +701,7 @@
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
     </row>
-    <row r="2" spans="2:26" ht="23.4" thickBot="1">
+    <row r="2" spans="2:26" ht="22.8">
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="5"/>
@@ -815,147 +726,152 @@
       <c r="W2" s="4"/>
       <c r="X2" s="4"/>
     </row>
-    <row r="3" spans="2:26" ht="48" customHeight="1">
-      <c r="B3" s="4"/>
-      <c r="C3" s="8" t="s">
+    <row r="3" spans="2:26" s="10" customFormat="1" ht="48" customHeight="1">
+      <c r="B3" s="9"/>
+      <c r="C3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="E3" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="17"/>
-      <c r="Y3" s="19" t="s">
+      <c r="Z3" s="12"/>
+    </row>
+    <row r="4" spans="2:26" s="10" customFormat="1" ht="65.25" customHeight="1">
+      <c r="B4" s="9"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Z3" s="20"/>
-    </row>
-    <row r="4" spans="2:26" ht="65.25" customHeight="1">
-      <c r="B4" s="4"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10" t="s">
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="10"/>
-      <c r="K4" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="L4" s="8"/>
-      <c r="M4" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10" t="s">
+      <c r="T4" s="11"/>
+      <c r="U4" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="V4" s="10"/>
-      <c r="W4" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="X4" s="17"/>
-      <c r="Y4" s="21"/>
-      <c r="Z4" s="22"/>
-    </row>
-    <row r="5" spans="2:26" ht="27.75" customHeight="1">
-      <c r="B5" s="4"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
-      <c r="V5" s="10"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="17"/>
-      <c r="Y5" s="21"/>
-      <c r="Z5" s="22"/>
-    </row>
-    <row r="6" spans="2:26" ht="14.4" thickBot="1">
-      <c r="B6" s="4"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="12"/>
+    </row>
+    <row r="5" spans="2:26" s="10" customFormat="1" ht="27.75" customHeight="1">
+      <c r="B5" s="9"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="11"/>
+      <c r="X5" s="11"/>
+      <c r="Y5" s="12"/>
+      <c r="Z5" s="12"/>
+    </row>
+    <row r="6" spans="2:26" s="10" customFormat="1">
+      <c r="B6" s="9"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="10"/>
-      <c r="W6" s="8"/>
-      <c r="X6" s="17"/>
-      <c r="Y6" s="23"/>
-      <c r="Z6" s="24"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="12"/>
+      <c r="Z6" s="12"/>
     </row>
     <row r="7" spans="2:26">
-      <c r="Y7" s="18"/>
+      <c r="Y7" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="E4:F6"/>
+    <mergeCell ref="G4:H5"/>
+    <mergeCell ref="I4:J6"/>
     <mergeCell ref="U4:V6"/>
     <mergeCell ref="W4:X6"/>
     <mergeCell ref="E3:X3"/>
@@ -965,80 +881,91 @@
     <mergeCell ref="O4:P5"/>
     <mergeCell ref="Q4:R6"/>
     <mergeCell ref="S4:T6"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="E4:F6"/>
-    <mergeCell ref="G4:H5"/>
-    <mergeCell ref="I4:J6"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="C2:AM6"/>
+  <dimension ref="B2:AM6"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="A7:XFD11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH4" sqref="AH4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1025" width="8.5" customWidth="1"/>
+    <col min="1" max="1" width="5.19921875" customWidth="1"/>
+    <col min="2" max="2" width="8.5" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="31.296875" customWidth="1"/>
+    <col min="4" max="4" width="16.3984375" customWidth="1"/>
+    <col min="5" max="5" width="14.296875" customWidth="1"/>
+    <col min="6" max="6" width="9.69921875" customWidth="1"/>
+    <col min="7" max="8" width="8.5" customWidth="1"/>
+    <col min="9" max="9" width="9.09765625" customWidth="1"/>
+    <col min="10" max="10" width="8.5" customWidth="1"/>
+    <col min="11" max="11" width="10.796875" customWidth="1"/>
+    <col min="12" max="12" width="8.5" customWidth="1"/>
+    <col min="13" max="13" width="11" customWidth="1"/>
+    <col min="14" max="30" width="8.5" customWidth="1"/>
+    <col min="31" max="31" width="12.296875" customWidth="1"/>
+    <col min="32" max="32" width="11.59765625" customWidth="1"/>
+    <col min="33" max="33" width="9.796875" customWidth="1"/>
+    <col min="34" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:39">
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11"/>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="11"/>
-      <c r="Z2" s="11"/>
-      <c r="AA2" s="11"/>
-      <c r="AB2" s="11"/>
-      <c r="AC2" s="11"/>
-      <c r="AD2" s="11"/>
-      <c r="AE2" s="11"/>
-      <c r="AF2" s="11"/>
-      <c r="AG2" s="11"/>
-      <c r="AH2" s="11"/>
-      <c r="AI2" s="11"/>
-      <c r="AJ2" s="11"/>
-      <c r="AK2" s="11"/>
-      <c r="AL2" s="11"/>
-      <c r="AM2" s="11"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="14"/>
+      <c r="AB2" s="14"/>
+      <c r="AC2" s="14"/>
+      <c r="AD2" s="14"/>
+      <c r="AE2" s="14"/>
+      <c r="AF2" s="14"/>
+      <c r="AG2" s="14"/>
+      <c r="AH2" s="14"/>
+      <c r="AI2" s="14"/>
+      <c r="AJ2" s="14"/>
+      <c r="AK2" s="14"/>
+      <c r="AL2" s="14"/>
+      <c r="AM2" s="14"/>
     </row>
     <row r="3" spans="3:39" ht="9.15" customHeight="1"/>
     <row r="4" spans="3:39" ht="31.35" customHeight="1">
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="13" t="s">
         <v>5</v>
       </c>
       <c r="H4" s="13" t="s">
@@ -1046,14 +973,14 @@
       </c>
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12" t="s">
+      <c r="L4" s="13"/>
+      <c r="M4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="12" t="s">
+      <c r="N4" s="13" t="s">
         <v>9</v>
       </c>
       <c r="O4" s="13" t="s">
@@ -1076,151 +1003,140 @@
         <v>11</v>
       </c>
       <c r="AD4" s="13"/>
-      <c r="AE4" s="12" t="s">
+      <c r="AE4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="AF4" s="12" t="s">
+      <c r="AF4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="AG4" s="12" t="s">
+      <c r="AG4" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="3:39" ht="14.25" customHeight="1">
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="3:39" ht="14.25" customHeight="1">
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12" t="s">
+      <c r="I5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="J5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="12" t="s">
+      <c r="L5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13" t="s">
         <v>18</v>
-      </c>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="13" t="s">
-        <v>19</v>
       </c>
       <c r="P5" s="13"/>
       <c r="Q5" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R5" s="13"/>
       <c r="S5" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="T5" s="13"/>
       <c r="U5" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V5" s="13"/>
       <c r="W5" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="X5" s="13"/>
       <c r="Y5" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Z5" s="13"/>
       <c r="AA5" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AB5" s="13"/>
       <c r="AC5" s="13"/>
       <c r="AD5" s="13"/>
-      <c r="AE5" s="12"/>
-      <c r="AF5" s="12"/>
-      <c r="AG5" s="12"/>
+      <c r="AE5" s="13"/>
+      <c r="AF5" s="13"/>
+      <c r="AG5" s="13"/>
     </row>
     <row r="6" spans="3:39" ht="73.95" customHeight="1">
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="6" t="s">
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="P6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="P6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q6" s="6" t="s">
+      <c r="Q6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="R6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="R6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="S6" s="6" t="s">
+      <c r="S6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="T6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="T6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="U6" s="6" t="s">
+      <c r="U6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="V6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="V6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="W6" s="6" t="s">
+      <c r="W6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="X6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="X6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y6" s="6" t="s">
+      <c r="Y6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="Z6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA6" s="6" t="s">
+      <c r="AA6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="AB6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="AC6" s="6" t="s">
+      <c r="AC6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="AD6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="AE6" s="12"/>
-      <c r="AF6" s="12"/>
-      <c r="AG6" s="12"/>
+      <c r="AE6" s="13"/>
+      <c r="AF6" s="13"/>
+      <c r="AG6" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="O5:P5"/>
     <mergeCell ref="I2:AM2"/>
     <mergeCell ref="C4:C6"/>
     <mergeCell ref="D4:D6"/>
@@ -1237,9 +1153,20 @@
     <mergeCell ref="AF4:AF6"/>
     <mergeCell ref="AG4:AG6"/>
     <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="Y5:Z5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1247,7 +1174,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -1258,79 +1185,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+    </row>
+    <row r="3" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A3" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-    </row>
-    <row r="3" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A3" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="13" t="s">
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13" t="s">
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+    </row>
+    <row r="5" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-    </row>
-    <row r="5" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13" t="s">
+      <c r="C5" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="D5" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="E5" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="13"/>
+      <c r="F5" s="16"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>27</v>
+      <c r="C6" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>